<commit_message>
Income distribution with ethnicity
</commit_message>
<xml_diff>
--- a/spring23-team-1/deliverables/deliverable2/Race_Income_Distribution.xlsx
+++ b/spring23-team-1/deliverables/deliverable2/Race_Income_Distribution.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65780803-4D3A-426B-B453-3F9CDEE4C4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D092D3-D9D4-4CE5-B7D1-6AB87C69A16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -238,28 +238,28 @@
     <t>Two or More Race</t>
   </si>
   <si>
-    <t>% White People</t>
-  </si>
-  <si>
-    <t>% American Indian and Alaska</t>
-  </si>
-  <si>
-    <t>% Asian</t>
-  </si>
-  <si>
-    <t>% Hawaiian</t>
-  </si>
-  <si>
-    <t>% Black/African</t>
-  </si>
-  <si>
-    <t>% Hispanic/Latino</t>
-  </si>
-  <si>
-    <t>% Other Races</t>
-  </si>
-  <si>
-    <t>% Two or More Races</t>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Black or African</t>
+  </si>
+  <si>
+    <t>American Indian &amp; Alaska</t>
+  </si>
+  <si>
+    <t>Asian Count</t>
+  </si>
+  <si>
+    <t>Native Hawaiian Count</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Two or More Ethnicity</t>
   </si>
 </sst>
 </file>
@@ -367,11 +367,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -773,16 +773,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
@@ -792,327 +792,362 @@
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11"/>
+      <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="10"/>
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" ht="25.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" spans="1:3" ht="51.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" spans="1:3" ht="89.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" spans="1:3" ht="25.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="11"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:3" ht="89.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" spans="1:3" ht="51.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:3" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="11"/>
+      <c r="C42" s="10"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="A43:C43"/>
@@ -1121,41 +1156,6 @@
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1175,10 +1175,10 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q4" sqref="Q4"/>
+      <selection pane="bottomRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,25 +1212,25 @@
         <v>64</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>65</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="J1" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>70</v>

</xml_diff>